<commit_message>
React Basics: List Rendering, useEffect examples are added
</commit_message>
<xml_diff>
--- a/DailyTest/5.5.25/sadaak-quiz-results_batch_DK.xlsx
+++ b/DailyTest/5.5.25/sadaak-quiz-results_batch_DK.xlsx
@@ -12,14 +12,15 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9780"/>
   </bookViews>
   <sheets>
-    <sheet name="online-quiz-app.results" sheetId="1" r:id="rId1"/>
+    <sheet name="6.6.25" sheetId="2" r:id="rId1"/>
+    <sheet name="5.5.25" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="169">
   <si>
     <t>S.NO</t>
   </si>
@@ -310,6 +311,222 @@
   </si>
   <si>
     <t>2025-05-05T09:45:13.956Z</t>
+  </si>
+  <si>
+    <t>ROLLNO</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:12:39.764Z</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:13:33.676Z</t>
+  </si>
+  <si>
+    <t>Ashwath K</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:13:43.166Z</t>
+  </si>
+  <si>
+    <t>M.mohamed tharik</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:14:21.787Z</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:14:52.577Z</t>
+  </si>
+  <si>
+    <t>suhail ahamed T</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:15:05.048Z</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:15:20.584Z</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:15:35.908Z</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:15:40.533Z</t>
+  </si>
+  <si>
+    <t>Syed Aakhil</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:16:15.776Z</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:16:25.845Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mohamed yusuf </t>
+  </si>
+  <si>
+    <t>2025-05-06T09:17:06.522Z</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:17:21.917Z</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:17:59.785Z</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:18:25.675Z</t>
+  </si>
+  <si>
+    <t>Hamdan Ashraf</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:18:44.724Z</t>
+  </si>
+  <si>
+    <t>sankara Narayanan S</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:18:59.240Z</t>
+  </si>
+  <si>
+    <t>abdalah</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:18:59.425Z</t>
+  </si>
+  <si>
+    <t>Brajin Sanu SA</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:19:51.993Z</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:20:06.714Z</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:20:10.500Z</t>
+  </si>
+  <si>
+    <t>Rajebul Ali</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:20:12.486Z</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:20:22.776Z</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:20:29.755Z</t>
+  </si>
+  <si>
+    <t>V.Bhuvaneshwari</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:21:06.811Z</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:21:23.094Z</t>
+  </si>
+  <si>
+    <t>surya</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:22:03.611Z</t>
+  </si>
+  <si>
+    <t>Ganesh.p</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:22:04.525Z</t>
+  </si>
+  <si>
+    <t>MUTHURAMAN G</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:22:05.531Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Santosh Mahara S </t>
+  </si>
+  <si>
+    <t>2025-05-06T09:22:14.795Z</t>
+  </si>
+  <si>
+    <t>Sakthivel V</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:22:16.504Z</t>
+  </si>
+  <si>
+    <t>chitharth M</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:22:32.577Z</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:23:35.728Z</t>
+  </si>
+  <si>
+    <t>dharnish</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:23:53.258Z</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:24:54.686Z</t>
+  </si>
+  <si>
+    <t>Syed Aahil R</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:24:56.061Z</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:25:16.923Z</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:25:59.203Z</t>
+  </si>
+  <si>
+    <t>Irfan Ahamed</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:25:59.697Z</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:26:21.592Z</t>
+  </si>
+  <si>
+    <t>A.Aafia Banu</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:26:31.186Z</t>
+  </si>
+  <si>
+    <t>Vinoth</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:27:23.006Z</t>
+  </si>
+  <si>
+    <t>Anas Rahman S</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:27:59.508Z</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:28:55.060Z</t>
+  </si>
+  <si>
+    <t>pradeep</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:29:47.864Z</t>
+  </si>
+  <si>
+    <t>mugesh.k</t>
+  </si>
+  <si>
+    <t>2025-05-06T09:35:11.332Z</t>
   </si>
 </sst>
 </file>
@@ -800,7 +1017,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -820,6 +1037,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -865,10 +1089,14 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="16">
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -878,11 +1106,33 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -893,7 +1143,97 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -949,6 +1289,35 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -991,15 +1360,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F46" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:F47" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F47"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="S.NO" dataDxfId="5"/>
+    <tableColumn id="2" name="NAME" dataDxfId="4"/>
+    <tableColumn id="3" name="DEPT" dataDxfId="3"/>
+    <tableColumn id="4" name="ROLLNO" dataDxfId="2"/>
+    <tableColumn id="5" name="SCORE" dataDxfId="1"/>
+    <tableColumn id="6" name="DATE" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F46" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="A1:F46"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="S.NO" dataDxfId="2"/>
-    <tableColumn id="2" name="NAME" dataDxfId="0"/>
-    <tableColumn id="3" name="ROLL NO" dataDxfId="1"/>
-    <tableColumn id="4" name="DEPT" dataDxfId="3"/>
-    <tableColumn id="5" name="SCORE" dataDxfId="5"/>
-    <tableColumn id="6" name="DATE" dataDxfId="4"/>
+    <tableColumn id="1" name="S.NO" dataDxfId="13"/>
+    <tableColumn id="2" name="NAME" dataDxfId="12"/>
+    <tableColumn id="3" name="ROLL NO" dataDxfId="11"/>
+    <tableColumn id="4" name="DEPT" dataDxfId="10"/>
+    <tableColumn id="5" name="SCORE" dataDxfId="9"/>
+    <tableColumn id="6" name="DATE" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1268,9 +1652,976 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.33203125" customWidth="1"/>
+    <col min="2" max="2" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5546875" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" customWidth="1"/>
+    <col min="6" max="6" width="25.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="8">
+        <v>311822104016</v>
+      </c>
+      <c r="E2" s="7">
+        <v>2</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="8">
+        <v>311822104005</v>
+      </c>
+      <c r="E3" s="7">
+        <v>14</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="8">
+        <v>311822104007</v>
+      </c>
+      <c r="E4" s="7">
+        <v>0</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="8">
+        <v>311822104034</v>
+      </c>
+      <c r="E5" s="7">
+        <v>4</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="8">
+        <v>311822104033</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="8">
+        <v>311822104049</v>
+      </c>
+      <c r="E7" s="7">
+        <v>8</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
+        <v>7</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="8">
+        <v>311822104027</v>
+      </c>
+      <c r="E8" s="7">
+        <v>7</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
+        <v>8</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="8">
+        <v>311822104032</v>
+      </c>
+      <c r="E9" s="7">
+        <v>10</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
+        <v>9</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="8">
+        <v>311822104304</v>
+      </c>
+      <c r="E10" s="7">
+        <v>9</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7">
+        <v>10</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="8">
+        <v>311822104052</v>
+      </c>
+      <c r="E11" s="7">
+        <v>2</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="7">
+        <v>11</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="8">
+        <v>311822104056</v>
+      </c>
+      <c r="E12" s="7">
+        <v>8</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
+        <v>12</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="8">
+        <v>311822104305</v>
+      </c>
+      <c r="E13" s="7">
+        <v>4</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="7">
+        <v>13</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="8">
+        <v>311822104025</v>
+      </c>
+      <c r="E14" s="7">
+        <v>7</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="7">
+        <v>14</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="8">
+        <v>311822104029</v>
+      </c>
+      <c r="E15" s="7">
+        <v>7</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="7">
+        <v>15</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="8">
+        <v>311822104303</v>
+      </c>
+      <c r="E16" s="7">
+        <v>5</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="7">
+        <v>16</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="8">
+        <v>311822104015</v>
+      </c>
+      <c r="E17" s="7">
+        <v>6</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="7">
+        <v>17</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="8">
+        <v>311822104043</v>
+      </c>
+      <c r="E18" s="7">
+        <v>8</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="7">
+        <v>18</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="8">
+        <v>311822104002</v>
+      </c>
+      <c r="E19" s="7">
+        <v>1</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="7">
+        <v>19</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="8">
+        <v>311822104009</v>
+      </c>
+      <c r="E20" s="7">
+        <v>14</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="7">
+        <v>20</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="8">
+        <v>311822104010</v>
+      </c>
+      <c r="E21" s="7">
+        <v>5</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="7">
+        <v>21</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="8">
+        <v>311822104004</v>
+      </c>
+      <c r="E22" s="7">
+        <v>7</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="7">
+        <v>22</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="8">
+        <v>311822104041</v>
+      </c>
+      <c r="E23" s="7">
+        <v>5</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="7">
+        <v>23</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="8">
+        <v>311822104030</v>
+      </c>
+      <c r="E24" s="7">
+        <v>13</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="7">
+        <v>24</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="8">
+        <v>311822104017</v>
+      </c>
+      <c r="E25" s="7">
+        <v>3</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="7">
+        <v>25</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="8">
+        <v>311822104008</v>
+      </c>
+      <c r="E26" s="7">
+        <v>8</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="7">
+        <v>26</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="8">
+        <v>311822104039</v>
+      </c>
+      <c r="E27" s="7">
+        <v>13</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="7">
+        <v>27</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="8">
+        <v>311822104050</v>
+      </c>
+      <c r="E28" s="7">
+        <v>0</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="7">
+        <v>28</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="8">
+        <v>311822104302</v>
+      </c>
+      <c r="E29" s="7">
+        <v>8</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="7">
+        <v>29</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="8">
+        <v>311822104038</v>
+      </c>
+      <c r="E30" s="7">
+        <v>12</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="7">
+        <v>30</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="8">
+        <v>311822104044</v>
+      </c>
+      <c r="E31" s="7">
+        <v>13</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="7">
+        <v>31</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="8">
+        <v>3118822104042</v>
+      </c>
+      <c r="E32" s="7">
+        <v>0</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="7">
+        <v>32</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="8">
+        <v>311822104011</v>
+      </c>
+      <c r="E33" s="7">
+        <v>6</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="7">
+        <v>33</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="8">
+        <v>311822104001</v>
+      </c>
+      <c r="E34" s="7">
+        <v>15</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="7">
+        <v>34</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="8">
+        <v>311822104013</v>
+      </c>
+      <c r="E35" s="7">
+        <v>7</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="7">
+        <v>35</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="8">
+        <v>311822104014</v>
+      </c>
+      <c r="E36" s="7">
+        <v>5</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="7">
+        <v>36</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="8">
+        <v>311822104051</v>
+      </c>
+      <c r="E37" s="7">
+        <v>15</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="7">
+        <v>37</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="8">
+        <v>311822104024</v>
+      </c>
+      <c r="E38" s="7">
+        <v>5</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="7">
+        <v>38</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" s="8">
+        <v>311822104045</v>
+      </c>
+      <c r="E39" s="7">
+        <v>1</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="7">
+        <v>39</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" s="8">
+        <v>311822104021</v>
+      </c>
+      <c r="E40" s="7">
+        <v>15</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="7">
+        <v>40</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="8">
+        <v>311822104022</v>
+      </c>
+      <c r="E41" s="7">
+        <v>15</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="7">
+        <v>41</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" s="8">
+        <v>311822104301</v>
+      </c>
+      <c r="E42" s="7">
+        <v>6</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="7">
+        <v>42</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" s="8">
+        <v>311822104054</v>
+      </c>
+      <c r="E43" s="7">
+        <v>4</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="7">
+        <v>43</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" s="8">
+        <v>311822104006</v>
+      </c>
+      <c r="E44" s="7">
+        <v>15</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="7">
+        <v>44</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" s="8">
+        <v>311822104019</v>
+      </c>
+      <c r="E45" s="7">
+        <v>13</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="7">
+        <v>45</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" s="8">
+        <v>311822104040</v>
+      </c>
+      <c r="E46" s="7">
+        <v>4</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="7">
+        <v>46</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" s="8">
+        <v>311822104037</v>
+      </c>
+      <c r="E47" s="7">
+        <v>6</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>